<commit_message>
Feat: Add more test cases to default commands excel file
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/exe_redfish/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC27045-4AAC-864A-A0DD-ED5326E4D388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EBA103-20BB-7149-BDBD-982E8FF4D8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Method</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>{"Password":"TestAABB!","TestKey3":"TestValue3","TestKey4":"TestValue4"}</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/testwronguser</t>
+  </si>
+  <si>
+    <t>{"UserName": "test3user", "password": "Test1234", "RoleId": "Administrator"}</t>
+  </si>
+  <si>
+    <t>{"UserName": "test2user", "Password": "Test1234", "RoleId": "Administrator","redundant-key":"redundant-value"}</t>
   </si>
 </sst>
 </file>
@@ -404,16 +413,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="40.6640625" customWidth="1"/>
-    <col min="3" max="3" width="73.6640625" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="88" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -448,24 +457,24 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -476,7 +485,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -487,15 +496,45 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: Add Delay Function
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EBA103-20BB-7149-BDBD-982E8FF4D8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E388E9-ADDB-3C4F-9DAB-5AB6EB9D5298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RedfishCommands" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>Method</t>
   </si>
@@ -74,6 +87,9 @@
   </si>
   <si>
     <t>{"UserName": "test2user", "Password": "Test1234", "RoleId": "Administrator","redundant-key":"redundant-value"}</t>
+  </si>
+  <si>
+    <t>DELAY</t>
   </si>
 </sst>
 </file>
@@ -413,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -537,6 +553,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Feat: Add ${username.id} to replace username with correct id
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E388E9-ADDB-3C4F-9DAB-5AB6EB9D5298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD5F84-BE85-1845-84F4-003E6FE928C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -62,9 +62,6 @@
     <t>PATCH</t>
   </si>
   <si>
-    <t>/redfish/v1/AccountService/Accounts/testuser</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>DELAY</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/${testuser.id}</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -479,7 +479,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -490,7 +490,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -498,10 +498,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -509,10 +509,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -520,10 +520,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -531,31 +531,31 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>10</v>

</xml_diff>

<commit_message>
Feat: Add more cases of recording user_name:user_id mapping
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD5F84-BE85-1845-84F4-003E6FE928C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0827C612-6543-EA42-958B-D89EECF9D67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>Method</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>/redfish/v1/AccountService/Accounts/${testuser.id}</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/1</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/admin</t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -462,24 +468,18 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -490,29 +490,29 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -523,7 +523,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -534,31 +534,53 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
-        <v>10</v>
+      <c r="B14">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: Add more test cases
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0827C612-6543-EA42-958B-D89EECF9D67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1BC392-09C9-8C4B-85E6-7BEFE140E0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t>Method</t>
   </si>
@@ -71,21 +71,12 @@
     <t>{"Password":"Test5678!"}</t>
   </si>
   <si>
-    <t>{"Password":"Test9012!","TestKey1":"TestValue1","TestKey2":"TestValue2"}</t>
-  </si>
-  <si>
     <t>{"Password":"TestAABB!","TestKey3":"TestValue3","TestKey4":"TestValue4"}</t>
   </si>
   <si>
     <t>/redfish/v1/AccountService/Accounts/testwronguser</t>
   </si>
   <si>
-    <t>{"UserName": "test3user", "password": "Test1234", "RoleId": "Administrator"}</t>
-  </si>
-  <si>
-    <t>{"UserName": "test2user", "Password": "Test1234", "RoleId": "Administrator","redundant-key":"redundant-value"}</t>
-  </si>
-  <si>
     <t>DELAY</t>
   </si>
   <si>
@@ -96,6 +87,45 @@
   </si>
   <si>
     <t>/redfish/v1/AccountService/Accounts/admin</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/${test2user.id}</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/${test3user.id}</t>
+  </si>
+  <si>
+    <t>{"Password":"Test9012!","TestKey1":"TestValue1","RoleId":"Operator"}</t>
+  </si>
+  <si>
+    <t>{"Password":"simplepasswordtest"}</t>
+  </si>
+  <si>
+    <t>{"Password":"Testxxxx!","TestKey1":"TestValue1"}</t>
+  </si>
+  <si>
+    <t>{"Password":"Test5678!","RoleId":"Manager"}</t>
+  </si>
+  <si>
+    <t>/redfish/v1/SessionService/Sessions</t>
+  </si>
+  <si>
+    <t>{"UserName": "test2user", "Password": "Test1234", "RoleId": "Administrator"}</t>
+  </si>
+  <si>
+    <t>{"UserName": "test3user", "Password": "Test1234", "RoleId": "Administrator","redundant-key":"redundant-value"}</t>
+  </si>
+  <si>
+    <t>{"UserName":"test2user","Password":"Test1234"}</t>
+  </si>
+  <si>
+    <t>{"Password":"Vveryvemmmmmmmmmmmmmmmmmmmmmmmmmryjjjjjjjjjjjjjjjjjjjjveryveryveryveryveryveryveryveryveryveryveryveryveryveryveryveryveryverylongpassword012!"}</t>
+  </si>
+  <si>
+    <t>{"Password":"aD0!"}</t>
+  </si>
+  <si>
+    <t>{"Password":"Test5678!","RoleId":"Manager","Testkey1":"testvalue"}</t>
   </si>
 </sst>
 </file>
@@ -131,8 +161,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -435,16 +468,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="43.5" customWidth="1"/>
-    <col min="3" max="3" width="88" customWidth="1"/>
+    <col min="3" max="3" width="144.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -471,7 +504,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -479,107 +512,235 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Feat: Add more test case
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1BC392-09C9-8C4B-85E6-7BEFE140E0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE7E60C-0EF9-9E4D-A8AF-DD7A6FAE3E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
   <si>
     <t>Method</t>
   </si>
@@ -126,6 +126,21 @@
   </si>
   <si>
     <t>{"Password":"Test5678!","RoleId":"Manager","Testkey1":"testvalue"}</t>
+  </si>
+  <si>
+    <t>{"UserName": "test5user", "Password": "Test1234!", "RoleId": "Administrator"}</t>
+  </si>
+  <si>
+    <t>{"PasswordChangeRequired":true}</t>
+  </si>
+  <si>
+    <t>{"UserName":"test5user","Password":"Test1234!"}</t>
+  </si>
+  <si>
+    <t>/redfish/v1/AccountService/Accounts/${test5user.id}</t>
+  </si>
+  <si>
+    <t>{"AccountLockoutThreshold":4}</t>
   </si>
 </sst>
 </file>
@@ -468,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -706,42 +721,94 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>7</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>14</v>
       </c>
-      <c r="B27">
-        <v>5</v>
+      <c r="B32">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat: Add test case
</commit_message>
<xml_diff>
--- a/commands.xlsx
+++ b/commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yoda/venus/redfish_agent/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE7E60C-0EF9-9E4D-A8AF-DD7A6FAE3E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E2E21AB-C40F-5744-B2FC-55FD3F4935D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>Method</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>{"AccountLockoutThreshold":4}</t>
+  </si>
+  <si>
+    <t>{"@odata.id": "/redfish/v1/AccountService/Accounts/rfpvbb6a/"}</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -556,13 +559,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -584,7 +584,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -595,18 +595,18 @@
         <v>5</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -617,7 +617,7 @@
         <v>15</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -628,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -639,7 +639,7 @@
         <v>15</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -650,7 +650,7 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -661,29 +661,29 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -694,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -705,7 +705,7 @@
         <v>15</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -716,40 +716,40 @@
         <v>15</v>
       </c>
       <c r="C22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
         <v>34</v>
       </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>33</v>
+      <c r="C25" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -757,26 +757,32 @@
         <v>8</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -784,7 +790,7 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -792,7 +798,7 @@
         <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -800,14 +806,30 @@
         <v>9</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>14</v>
       </c>
-      <c r="B32">
+      <c r="B34">
         <v>3</v>
       </c>
     </row>

</xml_diff>